<commit_message>
DSM#008 - Creating Commits' model and extraction
</commit_message>
<xml_diff>
--- a/src/data/resources/selected_repositories.xlsx
+++ b/src/data/resources/selected_repositories.xlsx
@@ -604,57 +604,57 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>virgili0</t>
+          <t>donnemartin</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Virgilio</t>
+          <t>data-science-ipython-notebooks</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>43536.78166666667</v>
+        <v>42027.81839120371</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>44488.26559027778</v>
+        <v>44504.84664351852</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>35112</v>
+        <v>49025</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Jupyter Notebook</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I3" t="n">
+        <v>12</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1627</v>
+      </c>
+      <c r="K3" t="n">
+        <v>21825</v>
+      </c>
+      <c r="L3" t="n">
+        <v>6809</v>
+      </c>
+      <c r="M3" t="n">
         <v>31</v>
       </c>
-      <c r="J3" t="n">
-        <v>785</v>
-      </c>
-      <c r="K3" t="n">
-        <v>13189</v>
-      </c>
-      <c r="L3" t="n">
-        <v>2509</v>
-      </c>
-      <c r="M3" t="n">
-        <v>37</v>
-      </c>
       <c r="N3" t="n">
-        <v>1363</v>
+        <v>543</v>
       </c>
       <c r="O3" t="n">
-        <v>123</v>
+        <v>53</v>
       </c>
       <c r="P3" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
@@ -664,32 +664,32 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Your new Mentor for Data Science E-Learning.</t>
+          <t>Data science Python notebooks: Deep learning (TensorFlow, Theano, Caffe, Keras), scikit-learn, Kaggle, big data (Spark, Hadoop MapReduce, HDFS), matplotlib, pandas, NumPy, SciPy, Python essentials, AWS, and various command lines.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>microsoft</t>
+          <t>virgili0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Data-Science-For-Beginners</t>
+          <t>Virgilio</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44258.68767361111</v>
+        <v>43536.78166666667</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>44519.76876157407</v>
+        <v>44488.26559027778</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>62297</v>
+        <v>35112</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -697,31 +697,31 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I4" t="n">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="J4" t="n">
-        <v>144</v>
+        <v>785</v>
       </c>
       <c r="K4" t="n">
-        <v>6991</v>
+        <v>13189</v>
       </c>
       <c r="L4" t="n">
-        <v>967</v>
+        <v>2509</v>
       </c>
       <c r="M4" t="n">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="N4" t="n">
-        <v>924</v>
+        <v>1363</v>
       </c>
       <c r="O4" t="n">
-        <v>215</v>
+        <v>123</v>
       </c>
       <c r="P4" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
@@ -731,32 +731,32 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>10 Weeks, 20 Lessons, Data Science for All!</t>
+          <t>Your new Mentor for Data Science E-Learning.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>firmai</t>
+          <t>microsoft</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>industry-machine-learning</t>
+          <t>Data-Science-For-Beginners</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>43588.2140625</v>
+        <v>44258.68767361111</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>44489.48476851852</v>
+        <v>44519.76876157407</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>3067</v>
+        <v>62297</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -764,28 +764,28 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I5" t="n">
-        <v>6</v>
+        <v>87</v>
       </c>
       <c r="J5" t="n">
-        <v>385</v>
+        <v>144</v>
       </c>
       <c r="K5" t="n">
-        <v>6065</v>
+        <v>6991</v>
       </c>
       <c r="L5" t="n">
-        <v>992</v>
+        <v>967</v>
       </c>
       <c r="M5" t="n">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="N5" t="n">
-        <v>157</v>
+        <v>924</v>
       </c>
       <c r="O5" t="n">
-        <v>5</v>
+        <v>215</v>
       </c>
       <c r="P5" t="n">
         <v>1</v>
@@ -798,64 +798,64 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>A curated list of applied machine learning and data science notebooks and libraries across different industries (by @firmai)</t>
+          <t>10 Weeks, 20 Lessons, Data Science for All!</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>fengdu78</t>
+          <t>joelgrus</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Data-Science-Notes</t>
+          <t>data-science-from-scratch</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>43675.16336805555</v>
+        <v>41952.10513888889</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>44424.47130787037</v>
+        <v>44313.96119212963</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>52628</v>
+        <v>769</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Jupyter Notebook</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J6" t="n">
-        <v>220</v>
+        <v>624</v>
       </c>
       <c r="K6" t="n">
-        <v>5960</v>
+        <v>6499</v>
       </c>
       <c r="L6" t="n">
-        <v>2595</v>
+        <v>3682</v>
       </c>
       <c r="M6" t="n">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="N6" t="n">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="O6" t="n">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="P6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
@@ -865,32 +865,32 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>数据科学的笔记以及资料搜集</t>
+          <t>code for Data Science From Scratch book</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>WillKoehrsen</t>
+          <t>firmai</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Data-Analysis</t>
+          <t>industry-machine-learning</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>42809.80076388889</v>
+        <v>43588.2140625</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44231.51909722222</v>
+        <v>44489.48476851852</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>376839</v>
+        <v>3067</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -898,31 +898,31 @@
         </is>
       </c>
       <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
         <v>6</v>
       </c>
-      <c r="I7" t="n">
-        <v>4</v>
-      </c>
       <c r="J7" t="n">
-        <v>350</v>
+        <v>385</v>
       </c>
       <c r="K7" t="n">
-        <v>4051</v>
+        <v>6065</v>
       </c>
       <c r="L7" t="n">
-        <v>3285</v>
+        <v>992</v>
       </c>
       <c r="M7" t="n">
-        <v>56</v>
+        <v>2</v>
       </c>
       <c r="N7" t="n">
-        <v>367</v>
+        <v>157</v>
       </c>
       <c r="O7" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="P7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -932,32 +932,32 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Data Science Using Python</t>
+          <t>A curated list of applied machine learning and data science notebooks and libraries across different industries (by @firmai)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>microsoft</t>
+          <t>fengdu78</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>tensorwatch</t>
+          <t>Data-Science-Notes</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>43600.35386574074</v>
+        <v>43675.16336805555</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>44299.40557870371</v>
+        <v>44424.47130787037</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>22242</v>
+        <v>52628</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -965,99 +965,99 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>104</v>
+        <v>220</v>
       </c>
       <c r="K8" t="n">
-        <v>3182</v>
+        <v>5960</v>
       </c>
       <c r="L8" t="n">
-        <v>346</v>
+        <v>2595</v>
       </c>
       <c r="M8" t="n">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="N8" t="n">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="O8" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="P8" t="n">
         <v>1</v>
       </c>
       <c r="Q8" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>Debugging, monitoring and visualization for Python Machine Learning and Data Science</t>
+          <t>数据科学的笔记以及资料搜集</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>nborwankar</t>
+          <t>rushter</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LearnDataScience</t>
+          <t>data-science-blogs</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>41481.10930555555</v>
+        <v>42221.49877314815</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>43760.41459490741</v>
+        <v>44411.99362268519</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>148439</v>
+        <v>348</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Jupyter Notebook</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
+        <v>86</v>
+      </c>
+      <c r="J9" t="n">
+        <v>470</v>
+      </c>
+      <c r="K9" t="n">
+        <v>5723</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1718</v>
+      </c>
+      <c r="M9" t="n">
         <v>7</v>
       </c>
-      <c r="J9" t="n">
-        <v>371</v>
-      </c>
-      <c r="K9" t="n">
-        <v>2673</v>
-      </c>
-      <c r="L9" t="n">
-        <v>1647</v>
-      </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
+        <v>359</v>
+      </c>
+      <c r="O9" t="n">
+        <v>114</v>
+      </c>
+      <c r="P9" t="n">
         <v>1</v>
       </c>
-      <c r="N9" t="n">
-        <v>64</v>
-      </c>
-      <c r="O9" t="n">
-        <v>19</v>
-      </c>
-      <c r="P9" t="n">
-        <v>2</v>
-      </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
@@ -1066,141 +1066,141 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Open Content for self-directed learning in data science</t>
+          <t>A curated list of data science blogs</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ml-tooling</t>
+          <t>drivendata</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ml-workspace</t>
+          <t>cookiecutter-data-science</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>43612.70503472222</v>
+        <v>42307.80552083333</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>44480.09324074074</v>
+        <v>44508.65208333333</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>13023</v>
+        <v>724</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Jupyter Notebook</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="H10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" t="n">
+        <v>45</v>
+      </c>
+      <c r="J10" t="n">
+        <v>98</v>
+      </c>
+      <c r="K10" t="n">
+        <v>5185</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1704</v>
+      </c>
+      <c r="M10" t="n">
+        <v>124</v>
+      </c>
+      <c r="N10" t="n">
+        <v>145</v>
+      </c>
+      <c r="O10" t="n">
+        <v>134</v>
+      </c>
+      <c r="P10" t="n">
         <v>7</v>
       </c>
-      <c r="I10" t="n">
-        <v>9</v>
-      </c>
-      <c r="J10" t="n">
-        <v>62</v>
-      </c>
-      <c r="K10" t="n">
-        <v>2287</v>
-      </c>
-      <c r="L10" t="n">
-        <v>314</v>
-      </c>
-      <c r="M10" t="n">
-        <v>73</v>
-      </c>
-      <c r="N10" t="n">
-        <v>845</v>
-      </c>
-      <c r="O10" t="n">
-        <v>29</v>
-      </c>
-      <c r="P10" t="n">
-        <v>4</v>
-      </c>
       <c r="Q10" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="R10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>🛠 All-in-one web-based IDE specialized for machine learning and data science.</t>
+          <t>A logical, reasonably standardized, but flexible project structure for doing and sharing data science work.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ShuaiW</t>
+          <t>Netflix</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>data-science-question-answer</t>
+          <t>metaflow</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>43115.06939814815</v>
+        <v>43725.74195601852</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>44105.20944444444</v>
+        <v>44519.87226851852</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>2390</v>
+        <v>9725</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Jupyter Notebook</t>
+          <t>Python</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I11" t="n">
-        <v>2</v>
+        <v>463</v>
       </c>
       <c r="J11" t="n">
-        <v>88</v>
+        <v>227</v>
       </c>
       <c r="K11" t="n">
-        <v>1980</v>
+        <v>4968</v>
       </c>
       <c r="L11" t="n">
-        <v>603</v>
+        <v>433</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>337</v>
       </c>
       <c r="N11" t="n">
-        <v>17</v>
+        <v>385</v>
       </c>
       <c r="O11" t="n">
-        <v>4</v>
+        <v>491</v>
       </c>
       <c r="P11" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>A repo for data science related questions and answers</t>
+          <t>:rocket: Build and manage real-life data science projects with ease!</t>
         </is>
       </c>
     </row>

</xml_diff>